<commit_message>
And change case 610 from 4 to 10
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MJWGit\ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C5FA36-DF8A-44B3-830B-A3A3A28B6EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E81626-3541-4B6B-A308-695050532C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2420,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AO579"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2982,7 +2982,7 @@
         <v>4.375</v>
       </c>
       <c r="D71" s="60">
-        <v>4.3330000000000002</v>
+        <v>10</v>
       </c>
       <c r="E71" s="56">
         <v>3.1920000000000002</v>

</xml_diff>